<commit_message>
added the 2018 Athens data to my own datasheet
</commit_message>
<xml_diff>
--- a/data/rrv_actigard_trial_2018_athens.xlsx
+++ b/data/rrv_actigard_trial_2018_athens.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/afife_ufl_edu/Documents/DISSERTATION/MANUSCRIPT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEFD901B-BD3D-4868-9FB2-7CAFE3664651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{DEFD901B-BD3D-4868-9FB2-7CAFE3664651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{928DFF00-C6D1-43FE-AD33-7C09308309AD}"/>
   <bookViews>
-    <workbookView xWindow="10215" yWindow="2040" windowWidth="9975" windowHeight="11385" xr2:uid="{3549144C-A5C3-423B-9A56-BA6D1BB115ED}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="12735" xr2:uid="{3549144C-A5C3-423B-9A56-BA6D1BB115ED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="mites" sheetId="1" r:id="rId1"/>
+    <sheet name="horsfield-barratt" sheetId="2" r:id="rId2"/>
+    <sheet name="audpc_totals" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="95">
   <si>
     <t>Watkinsville, GA</t>
   </si>
@@ -241,18 +243,103 @@
   </si>
   <si>
     <t>Sample #</t>
+  </si>
+  <si>
+    <t>Mid point values</t>
+  </si>
+  <si>
+    <t>Week 1</t>
+  </si>
+  <si>
+    <t>Week 2</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t>Week 7</t>
+  </si>
+  <si>
+    <t>Week 8</t>
+  </si>
+  <si>
+    <t>Week 9</t>
+  </si>
+  <si>
+    <t>Week 10</t>
+  </si>
+  <si>
+    <t>Week 17</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>Rep</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Non-inoc</t>
+  </si>
+  <si>
+    <t>AUDPC</t>
+  </si>
+  <si>
+    <t>Final disease severity (%)</t>
+  </si>
+  <si>
+    <t>Number of infected plants</t>
+  </si>
+  <si>
+    <t>Non-treated</t>
+  </si>
+  <si>
+    <t>ASM - LR</t>
+  </si>
+  <si>
+    <t>ASM -HR</t>
+  </si>
+  <si>
+    <t>NI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -276,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -284,6 +371,14 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F10B9E-D491-4EDC-B482-8B21AD6D2BB6}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1702,4 +1797,2347 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B756A610-8B74-4B0B-B5E6-7C45A7DD1112}">
+  <dimension ref="A1:O51"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="5">
+        <v>43343</v>
+      </c>
+      <c r="D1" s="5">
+        <v>43350</v>
+      </c>
+      <c r="E1" s="5">
+        <v>43357</v>
+      </c>
+      <c r="F1" s="5">
+        <v>43364</v>
+      </c>
+      <c r="G1" s="6">
+        <v>43371</v>
+      </c>
+      <c r="H1" s="6">
+        <v>43378</v>
+      </c>
+      <c r="I1" s="6">
+        <v>43385</v>
+      </c>
+      <c r="J1" s="6">
+        <v>43392</v>
+      </c>
+      <c r="K1" s="6">
+        <v>43399</v>
+      </c>
+      <c r="L1" s="6">
+        <v>43406</v>
+      </c>
+      <c r="M1" s="6">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" t="s">
+        <v>88</v>
+      </c>
+      <c r="O2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="N3">
+        <v>124.25</v>
+      </c>
+      <c r="O3">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="J4" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K4" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="L4" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M4" s="4">
+        <v>17.5</v>
+      </c>
+      <c r="N4">
+        <v>52.5</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="4">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K5" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="L5" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>57.75</v>
+      </c>
+      <c r="O5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K6" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M6" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="N6">
+        <v>31.5</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="J7" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>52.5</v>
+      </c>
+      <c r="O7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="J8" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="4">
+        <v>9</v>
+      </c>
+      <c r="N8">
+        <v>73.5</v>
+      </c>
+      <c r="O8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="J9" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K9" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L9" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M9" s="4">
+        <v>9</v>
+      </c>
+      <c r="N9">
+        <v>26.25</v>
+      </c>
+      <c r="O9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L10" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M10" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="N10">
+        <v>36.75</v>
+      </c>
+      <c r="O10">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L11" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M11" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="N11">
+        <v>42</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <v>9</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="J12" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K12" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L12" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>31.5</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="4">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K13" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L13" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>36.75</v>
+      </c>
+      <c r="O13">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>11</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L14" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M14" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="N14">
+        <v>103.25</v>
+      </c>
+      <c r="O14">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="J15" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K15" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M15" s="4">
+        <v>17.5</v>
+      </c>
+      <c r="N15">
+        <v>52.5</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0</v>
+      </c>
+      <c r="J16" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K16" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="L16" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>36.75</v>
+      </c>
+      <c r="O16">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="4">
+        <v>2</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L17" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M17" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="N17">
+        <v>78.75</v>
+      </c>
+      <c r="O17">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <v>3</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="J18" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K18" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="L18" s="4">
+        <v>0</v>
+      </c>
+      <c r="M18" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="N18">
+        <v>36.75</v>
+      </c>
+      <c r="O18">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B19" s="4">
+        <v>4</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="I19" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="J19" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K19" s="4">
+        <v>0</v>
+      </c>
+      <c r="L19" s="4">
+        <v>0</v>
+      </c>
+      <c r="M19" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="N19">
+        <v>82.25</v>
+      </c>
+      <c r="O19">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="4">
+        <v>5</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0</v>
+      </c>
+      <c r="H20" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0</v>
+      </c>
+      <c r="J20" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K20" s="4">
+        <v>0</v>
+      </c>
+      <c r="L20" s="4">
+        <v>0</v>
+      </c>
+      <c r="M20" s="4">
+        <v>17.5</v>
+      </c>
+      <c r="N20">
+        <v>42</v>
+      </c>
+      <c r="O20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="4">
+        <v>6</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0</v>
+      </c>
+      <c r="K21" s="4">
+        <v>0</v>
+      </c>
+      <c r="L21" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M21" s="4">
+        <v>9</v>
+      </c>
+      <c r="N21">
+        <v>113.75</v>
+      </c>
+      <c r="O21">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
+        <v>7</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G22" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="H22" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="I22" s="4">
+        <v>0</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0</v>
+      </c>
+      <c r="K22" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L22" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M22" s="4">
+        <v>17.5</v>
+      </c>
+      <c r="N22">
+        <v>99.75</v>
+      </c>
+      <c r="O22">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="4">
+        <v>8</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="H23" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="I23" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="J23" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K23" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L23" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M23" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="N23">
+        <v>71.75</v>
+      </c>
+      <c r="O23">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
+        <v>9</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0</v>
+      </c>
+      <c r="G24" s="4">
+        <v>0</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0</v>
+      </c>
+      <c r="I24" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="J24" s="4">
+        <v>0</v>
+      </c>
+      <c r="K24" s="4">
+        <v>0</v>
+      </c>
+      <c r="L24" s="4">
+        <v>0</v>
+      </c>
+      <c r="M24" s="4">
+        <v>17.5</v>
+      </c>
+      <c r="N24">
+        <v>47.25</v>
+      </c>
+      <c r="O24">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
+        <v>10</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0</v>
+      </c>
+      <c r="I25" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="J25" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K25" s="4">
+        <v>0</v>
+      </c>
+      <c r="L25" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M25" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="N25">
+        <v>52.5</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B26" s="4">
+        <v>11</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0</v>
+      </c>
+      <c r="G26" s="4">
+        <v>0</v>
+      </c>
+      <c r="H26" s="4">
+        <v>0</v>
+      </c>
+      <c r="I26" s="4">
+        <v>0</v>
+      </c>
+      <c r="J26" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K26" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="L26" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M26" s="4">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>36.75</v>
+      </c>
+      <c r="O26">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="4">
+        <v>12</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0</v>
+      </c>
+      <c r="F27" s="4">
+        <v>0</v>
+      </c>
+      <c r="G27" s="4">
+        <v>0</v>
+      </c>
+      <c r="H27" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="I27" s="4">
+        <v>0</v>
+      </c>
+      <c r="J27" s="4">
+        <v>0</v>
+      </c>
+      <c r="K27" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L27" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M27" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="N27">
+        <v>78.75</v>
+      </c>
+      <c r="O27">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="4">
+        <v>1</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4">
+        <v>0</v>
+      </c>
+      <c r="G28" s="4">
+        <v>0</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0</v>
+      </c>
+      <c r="I28" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="J28" s="4">
+        <v>0</v>
+      </c>
+      <c r="K28" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="L28" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="M28" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="N28">
+        <v>71.75</v>
+      </c>
+      <c r="O28">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="4">
+        <v>2</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0</v>
+      </c>
+      <c r="G29" s="4">
+        <v>0</v>
+      </c>
+      <c r="H29" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="I29" s="4">
+        <v>0</v>
+      </c>
+      <c r="J29" s="4">
+        <v>0</v>
+      </c>
+      <c r="K29" s="4">
+        <v>0</v>
+      </c>
+      <c r="L29" s="4">
+        <v>0</v>
+      </c>
+      <c r="M29" s="4">
+        <v>17.5</v>
+      </c>
+      <c r="N29">
+        <v>103.25</v>
+      </c>
+      <c r="O29">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="4">
+        <v>3</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0</v>
+      </c>
+      <c r="G30" s="4">
+        <v>0</v>
+      </c>
+      <c r="H30" s="4">
+        <v>0</v>
+      </c>
+      <c r="I30" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="J30" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K30" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L30" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M30" s="4">
+        <v>17.5</v>
+      </c>
+      <c r="N30">
+        <v>26.25</v>
+      </c>
+      <c r="O30">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B31" s="4">
+        <v>4</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0</v>
+      </c>
+      <c r="D31" s="4">
+        <v>0</v>
+      </c>
+      <c r="E31" s="4">
+        <v>0</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0</v>
+      </c>
+      <c r="G31" s="4">
+        <v>0</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0</v>
+      </c>
+      <c r="I31" s="4">
+        <v>0</v>
+      </c>
+      <c r="J31" s="4">
+        <v>0</v>
+      </c>
+      <c r="K31" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L31" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M31" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="N31">
+        <v>47.25</v>
+      </c>
+      <c r="O31">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B32" s="4">
+        <v>5</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0</v>
+      </c>
+      <c r="E32" s="4">
+        <v>0</v>
+      </c>
+      <c r="F32" s="4">
+        <v>0</v>
+      </c>
+      <c r="G32" s="4">
+        <v>0</v>
+      </c>
+      <c r="H32" s="4">
+        <v>0</v>
+      </c>
+      <c r="I32" s="4">
+        <v>0</v>
+      </c>
+      <c r="J32" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K32" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L32" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M32" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="N32">
+        <v>31.5</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B33" s="4">
+        <v>6</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0</v>
+      </c>
+      <c r="E33" s="4">
+        <v>0</v>
+      </c>
+      <c r="F33" s="4">
+        <v>0</v>
+      </c>
+      <c r="G33" s="4">
+        <v>0</v>
+      </c>
+      <c r="H33" s="4">
+        <v>0</v>
+      </c>
+      <c r="I33" s="4">
+        <v>0</v>
+      </c>
+      <c r="J33" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K33" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L33" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M33" s="4">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>26.25</v>
+      </c>
+      <c r="O33">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B34" s="4">
+        <v>7</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0</v>
+      </c>
+      <c r="E34" s="4">
+        <v>0</v>
+      </c>
+      <c r="F34" s="4">
+        <v>0</v>
+      </c>
+      <c r="G34" s="4">
+        <v>0</v>
+      </c>
+      <c r="H34" s="4">
+        <v>0</v>
+      </c>
+      <c r="I34" s="4">
+        <v>0</v>
+      </c>
+      <c r="J34" s="4">
+        <v>0</v>
+      </c>
+      <c r="K34" s="4">
+        <v>0</v>
+      </c>
+      <c r="L34" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M34" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="N34">
+        <v>334.25</v>
+      </c>
+      <c r="O34">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B35" s="4">
+        <v>8</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0</v>
+      </c>
+      <c r="E35" s="4">
+        <v>0</v>
+      </c>
+      <c r="F35" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G35" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="H35" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="I35" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="J35" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K35" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="L35" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="M35" s="4">
+        <v>62.5</v>
+      </c>
+      <c r="N35">
+        <v>103.25</v>
+      </c>
+      <c r="O35">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B36" s="4">
+        <v>9</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0</v>
+      </c>
+      <c r="E36" s="4">
+        <v>0</v>
+      </c>
+      <c r="F36" s="4">
+        <v>0</v>
+      </c>
+      <c r="G36" s="4">
+        <v>0</v>
+      </c>
+      <c r="H36" s="4">
+        <v>0</v>
+      </c>
+      <c r="I36" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="J36" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K36" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L36" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M36" s="4">
+        <v>17.5</v>
+      </c>
+      <c r="N36">
+        <v>42</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B37" s="4">
+        <v>10</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0</v>
+      </c>
+      <c r="E37" s="4">
+        <v>0</v>
+      </c>
+      <c r="F37" s="4">
+        <v>0</v>
+      </c>
+      <c r="G37" s="4">
+        <v>0</v>
+      </c>
+      <c r="H37" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="I37" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="J37" s="4">
+        <v>0</v>
+      </c>
+      <c r="K37" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L37" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M37" s="4">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>5.25</v>
+      </c>
+      <c r="O37">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B38" s="4">
+        <v>11</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0</v>
+      </c>
+      <c r="D38" s="4">
+        <v>0</v>
+      </c>
+      <c r="E38" s="4">
+        <v>0</v>
+      </c>
+      <c r="F38" s="4">
+        <v>0</v>
+      </c>
+      <c r="G38" s="4">
+        <v>0</v>
+      </c>
+      <c r="H38" s="4">
+        <v>0</v>
+      </c>
+      <c r="I38" s="4">
+        <v>0</v>
+      </c>
+      <c r="J38" s="4">
+        <v>0</v>
+      </c>
+      <c r="K38" s="4">
+        <v>0</v>
+      </c>
+      <c r="L38" s="4">
+        <v>0</v>
+      </c>
+      <c r="M38" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="N38">
+        <v>10.5</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B39" s="4">
+        <v>12</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0</v>
+      </c>
+      <c r="E39" s="4">
+        <v>0</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0</v>
+      </c>
+      <c r="G39" s="4">
+        <v>0</v>
+      </c>
+      <c r="H39" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="I39" s="4">
+        <v>0</v>
+      </c>
+      <c r="J39" s="4">
+        <v>0</v>
+      </c>
+      <c r="K39" s="4">
+        <v>0</v>
+      </c>
+      <c r="L39" s="4">
+        <v>0</v>
+      </c>
+      <c r="M39" s="4">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="4">
+        <v>1</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0</v>
+      </c>
+      <c r="D40" s="4">
+        <v>0</v>
+      </c>
+      <c r="E40" s="4">
+        <v>0</v>
+      </c>
+      <c r="F40" s="4">
+        <v>0</v>
+      </c>
+      <c r="G40" s="4">
+        <v>0</v>
+      </c>
+      <c r="H40" s="4">
+        <v>0</v>
+      </c>
+      <c r="I40" s="4">
+        <v>0</v>
+      </c>
+      <c r="J40" s="4">
+        <v>0</v>
+      </c>
+      <c r="K40" s="4">
+        <v>0</v>
+      </c>
+      <c r="L40" s="4">
+        <v>0</v>
+      </c>
+      <c r="M40" s="4">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>5.25</v>
+      </c>
+      <c r="O40">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B41" s="4">
+        <v>2</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0</v>
+      </c>
+      <c r="E41" s="4">
+        <v>0</v>
+      </c>
+      <c r="F41" s="4">
+        <v>0</v>
+      </c>
+      <c r="G41" s="4">
+        <v>0</v>
+      </c>
+      <c r="H41" s="4">
+        <v>0</v>
+      </c>
+      <c r="I41" s="4">
+        <v>0</v>
+      </c>
+      <c r="J41" s="4">
+        <v>0</v>
+      </c>
+      <c r="K41" s="4">
+        <v>0</v>
+      </c>
+      <c r="L41" s="4">
+        <v>0</v>
+      </c>
+      <c r="M41" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B42" s="4">
+        <v>3</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0</v>
+      </c>
+      <c r="E42" s="4">
+        <v>0</v>
+      </c>
+      <c r="F42" s="4">
+        <v>0</v>
+      </c>
+      <c r="G42" s="4">
+        <v>0</v>
+      </c>
+      <c r="H42" s="4">
+        <v>0</v>
+      </c>
+      <c r="I42" s="4">
+        <v>0</v>
+      </c>
+      <c r="J42" s="4">
+        <v>0</v>
+      </c>
+      <c r="K42" s="4">
+        <v>0</v>
+      </c>
+      <c r="L42" s="4">
+        <v>0</v>
+      </c>
+      <c r="M42" s="4">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>5.25</v>
+      </c>
+      <c r="O42">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B43" s="4">
+        <v>4</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0</v>
+      </c>
+      <c r="D43" s="4">
+        <v>0</v>
+      </c>
+      <c r="E43" s="4">
+        <v>0</v>
+      </c>
+      <c r="F43" s="4">
+        <v>0</v>
+      </c>
+      <c r="G43" s="4">
+        <v>0</v>
+      </c>
+      <c r="H43" s="4">
+        <v>0</v>
+      </c>
+      <c r="I43" s="4">
+        <v>0</v>
+      </c>
+      <c r="J43" s="4">
+        <v>0</v>
+      </c>
+      <c r="K43" s="4">
+        <v>0</v>
+      </c>
+      <c r="L43" s="4">
+        <v>0</v>
+      </c>
+      <c r="M43" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B44" s="4">
+        <v>5</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0</v>
+      </c>
+      <c r="D44" s="4">
+        <v>0</v>
+      </c>
+      <c r="E44" s="4">
+        <v>0</v>
+      </c>
+      <c r="F44" s="4">
+        <v>0</v>
+      </c>
+      <c r="G44" s="4">
+        <v>0</v>
+      </c>
+      <c r="H44" s="4">
+        <v>0</v>
+      </c>
+      <c r="I44" s="4">
+        <v>0</v>
+      </c>
+      <c r="J44" s="4">
+        <v>0</v>
+      </c>
+      <c r="K44" s="4">
+        <v>0</v>
+      </c>
+      <c r="L44" s="4">
+        <v>0</v>
+      </c>
+      <c r="M44" s="4">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B45" s="4">
+        <v>6</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0</v>
+      </c>
+      <c r="E45" s="4">
+        <v>0</v>
+      </c>
+      <c r="F45" s="4">
+        <v>0</v>
+      </c>
+      <c r="G45" s="4">
+        <v>0</v>
+      </c>
+      <c r="H45" s="4">
+        <v>0</v>
+      </c>
+      <c r="I45" s="4">
+        <v>0</v>
+      </c>
+      <c r="J45" s="4">
+        <v>0</v>
+      </c>
+      <c r="K45" s="4">
+        <v>0</v>
+      </c>
+      <c r="L45" s="4">
+        <v>0</v>
+      </c>
+      <c r="M45" s="4">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B46" s="4">
+        <v>7</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0</v>
+      </c>
+      <c r="E46" s="4">
+        <v>0</v>
+      </c>
+      <c r="F46" s="4">
+        <v>0</v>
+      </c>
+      <c r="G46" s="4">
+        <v>0</v>
+      </c>
+      <c r="H46" s="4">
+        <v>0</v>
+      </c>
+      <c r="I46" s="4">
+        <v>0</v>
+      </c>
+      <c r="J46" s="4">
+        <v>0</v>
+      </c>
+      <c r="K46" s="4">
+        <v>0</v>
+      </c>
+      <c r="L46" s="4">
+        <v>0</v>
+      </c>
+      <c r="M46" s="4">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B47" s="4">
+        <v>8</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0</v>
+      </c>
+      <c r="E47" s="4">
+        <v>0</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0</v>
+      </c>
+      <c r="G47" s="4">
+        <v>0</v>
+      </c>
+      <c r="H47" s="4">
+        <v>0</v>
+      </c>
+      <c r="I47" s="4">
+        <v>0</v>
+      </c>
+      <c r="J47" s="4">
+        <v>0</v>
+      </c>
+      <c r="K47" s="4">
+        <v>0</v>
+      </c>
+      <c r="L47" s="4">
+        <v>0</v>
+      </c>
+      <c r="M47" s="4">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B48" s="4">
+        <v>9</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0</v>
+      </c>
+      <c r="E48" s="4">
+        <v>0</v>
+      </c>
+      <c r="F48" s="4">
+        <v>0</v>
+      </c>
+      <c r="G48" s="4">
+        <v>0</v>
+      </c>
+      <c r="H48" s="4">
+        <v>0</v>
+      </c>
+      <c r="I48" s="4">
+        <v>0</v>
+      </c>
+      <c r="J48" s="4">
+        <v>0</v>
+      </c>
+      <c r="K48" s="4">
+        <v>0</v>
+      </c>
+      <c r="L48" s="4">
+        <v>0</v>
+      </c>
+      <c r="M48" s="4">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>5.25</v>
+      </c>
+      <c r="O48">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B49" s="4">
+        <v>10</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0</v>
+      </c>
+      <c r="D49" s="4">
+        <v>0</v>
+      </c>
+      <c r="E49" s="4">
+        <v>0</v>
+      </c>
+      <c r="F49" s="4">
+        <v>0</v>
+      </c>
+      <c r="G49" s="4">
+        <v>0</v>
+      </c>
+      <c r="H49" s="4">
+        <v>0</v>
+      </c>
+      <c r="I49" s="4">
+        <v>0</v>
+      </c>
+      <c r="J49" s="4">
+        <v>0</v>
+      </c>
+      <c r="K49" s="4">
+        <v>0</v>
+      </c>
+      <c r="L49" s="4">
+        <v>0</v>
+      </c>
+      <c r="M49" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B50" s="4">
+        <v>11</v>
+      </c>
+      <c r="C50" s="4">
+        <v>0</v>
+      </c>
+      <c r="D50" s="4">
+        <v>0</v>
+      </c>
+      <c r="E50" s="4">
+        <v>0</v>
+      </c>
+      <c r="F50" s="4">
+        <v>0</v>
+      </c>
+      <c r="G50" s="4">
+        <v>0</v>
+      </c>
+      <c r="H50" s="4">
+        <v>0</v>
+      </c>
+      <c r="I50" s="4">
+        <v>0</v>
+      </c>
+      <c r="J50" s="4">
+        <v>0</v>
+      </c>
+      <c r="K50" s="4">
+        <v>0</v>
+      </c>
+      <c r="L50" s="4">
+        <v>0</v>
+      </c>
+      <c r="M50" s="4">
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B51" s="4">
+        <v>12</v>
+      </c>
+      <c r="C51" s="4">
+        <v>0</v>
+      </c>
+      <c r="D51" s="4">
+        <v>0</v>
+      </c>
+      <c r="E51" s="4">
+        <v>0</v>
+      </c>
+      <c r="F51" s="4">
+        <v>0</v>
+      </c>
+      <c r="G51" s="4">
+        <v>0</v>
+      </c>
+      <c r="H51" s="4">
+        <v>0</v>
+      </c>
+      <c r="I51" s="4">
+        <v>0</v>
+      </c>
+      <c r="J51" s="4">
+        <v>0</v>
+      </c>
+      <c r="K51" s="4">
+        <v>0</v>
+      </c>
+      <c r="L51" s="4">
+        <v>0</v>
+      </c>
+      <c r="M51" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C0A11F1-13A9-43A9-BE96-E16FF082F3B0}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2">
+        <v>55.708333333333336</v>
+      </c>
+      <c r="C2">
+        <v>5.166666666666667</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3">
+        <v>62.5625</v>
+      </c>
+      <c r="C3">
+        <v>6.625</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4">
+        <v>73.354166666666671</v>
+      </c>
+      <c r="C4">
+        <v>10.708333333333334</v>
+      </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5">
+        <v>1.3125</v>
+      </c>
+      <c r="C5">
+        <v>0.375</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
I couldn't handle it, I had to do some manual editing of column names and in Excel to make the file easier to read into R
</commit_message>
<xml_diff>
--- a/data/rrv_actigard_trial_2018_athens.xlsx
+++ b/data/rrv_actigard_trial_2018_athens.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/afife_ufl_edu/Documents/DISSERTATION/MANUSCRIPT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{DEFD901B-BD3D-4868-9FB2-7CAFE3664651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{928DFF00-C6D1-43FE-AD33-7C09308309AD}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{DEFD901B-BD3D-4868-9FB2-7CAFE3664651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FA95C7B-3355-438C-A437-64983A2CACC7}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="12735" xr2:uid="{3549144C-A5C3-423B-9A56-BA6D1BB115ED}"/>
+    <workbookView xWindow="7200" yWindow="4665" windowWidth="21600" windowHeight="12735" activeTab="1" xr2:uid="{3549144C-A5C3-423B-9A56-BA6D1BB115ED}"/>
   </bookViews>
   <sheets>
     <sheet name="mites" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="94">
   <si>
     <t>Watkinsville, GA</t>
   </si>
@@ -285,9 +285,6 @@
   </si>
   <si>
     <t>Rep</t>
-  </si>
-  <si>
-    <t>Rating</t>
   </si>
   <si>
     <t>Water</t>
@@ -695,7 +692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F10B9E-D491-4EDC-B482-8B21AD6D2BB6}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -1801,13 +1798,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B756A610-8B74-4B0B-B5E6-7C45A7DD1112}">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -1849,7 +1854,12 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="4"/>
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="C2" s="4" t="s">
         <v>70</v>
       </c>
@@ -1884,51 +1894,51 @@
         <v>80</v>
       </c>
       <c r="N2" t="s">
+        <v>87</v>
+      </c>
+      <c r="O2" t="s">
         <v>88</v>
-      </c>
-      <c r="O2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>83</v>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K3" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="L3" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M3" s="4">
+        <v>17.5</v>
       </c>
       <c r="N3">
         <v>124.25</v>
@@ -1939,10 +1949,10 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="4">
         <v>0</v>
@@ -1963,7 +1973,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="J4" s="4">
         <v>1.5</v>
@@ -1975,7 +1985,7 @@
         <v>1.5</v>
       </c>
       <c r="M4" s="4">
-        <v>17.5</v>
+        <v>0</v>
       </c>
       <c r="N4">
         <v>52.5</v>
@@ -1985,8 +1995,11 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
       <c r="B5" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="4">
         <v>0</v>
@@ -2019,7 +2032,7 @@
         <v>1.5</v>
       </c>
       <c r="M5" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="N5">
         <v>57.75</v>
@@ -2029,8 +2042,11 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
       <c r="B6" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="4">
         <v>0</v>
@@ -2051,19 +2067,19 @@
         <v>0</v>
       </c>
       <c r="I6" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="J6" s="4">
         <v>1.5</v>
       </c>
       <c r="K6" s="4">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="L6" s="4">
         <v>1.5</v>
       </c>
       <c r="M6" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="N6">
         <v>31.5</v>
@@ -2073,8 +2089,11 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
       <c r="B7" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="4">
         <v>0</v>
@@ -2104,10 +2123,10 @@
         <v>0</v>
       </c>
       <c r="L7" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="M7" s="4">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="N7">
         <v>52.5</v>
@@ -2117,8 +2136,11 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
       <c r="B8" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="4">
         <v>0</v>
@@ -2145,10 +2167,10 @@
         <v>1.5</v>
       </c>
       <c r="K8" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="L8" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="M8" s="4">
         <v>9</v>
@@ -2161,8 +2183,11 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
       <c r="B9" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="4">
         <v>0</v>
@@ -2183,10 +2208,10 @@
         <v>0</v>
       </c>
       <c r="I9" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="J9" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="K9" s="4">
         <v>1.5</v>
@@ -2195,7 +2220,7 @@
         <v>1.5</v>
       </c>
       <c r="M9" s="4">
-        <v>9</v>
+        <v>1.5</v>
       </c>
       <c r="N9">
         <v>26.25</v>
@@ -2205,8 +2230,11 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>83</v>
+      </c>
       <c r="B10" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="4">
         <v>0</v>
@@ -2239,7 +2267,7 @@
         <v>1.5</v>
       </c>
       <c r="M10" s="4">
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="N10">
         <v>36.75</v>
@@ -2249,8 +2277,11 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
       <c r="B11" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11" s="4">
         <v>0</v>
@@ -2271,10 +2302,10 @@
         <v>0</v>
       </c>
       <c r="I11" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="J11" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K11" s="4">
         <v>1.5</v>
@@ -2283,7 +2314,7 @@
         <v>1.5</v>
       </c>
       <c r="M11" s="4">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="N11">
         <v>42</v>
@@ -2293,8 +2324,11 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
       <c r="B12" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" s="4">
         <v>0</v>
@@ -2315,7 +2349,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="J12" s="4">
         <v>1.5</v>
@@ -2337,8 +2371,11 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
       <c r="B13" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="4">
         <v>0</v>
@@ -2356,13 +2393,13 @@
         <v>0</v>
       </c>
       <c r="H13" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I13" s="4">
         <v>0</v>
       </c>
       <c r="J13" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="K13" s="4">
         <v>1.5</v>
@@ -2371,7 +2408,7 @@
         <v>1.5</v>
       </c>
       <c r="M13" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="N13">
         <v>36.75</v>
@@ -2381,8 +2418,11 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>83</v>
+      </c>
       <c r="B14" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C14" s="4">
         <v>0</v>
@@ -2400,13 +2440,13 @@
         <v>0</v>
       </c>
       <c r="H14" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="I14" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="J14" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K14" s="4">
         <v>1.5</v>
@@ -2415,7 +2455,7 @@
         <v>1.5</v>
       </c>
       <c r="M14" s="4">
-        <v>1.5</v>
+        <v>17.5</v>
       </c>
       <c r="N14">
         <v>103.25</v>
@@ -2425,8 +2465,11 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>84</v>
+      </c>
       <c r="B15" s="4">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C15" s="4">
         <v>0</v>
@@ -2447,19 +2490,19 @@
         <v>0</v>
       </c>
       <c r="I15" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="J15" s="4">
         <v>1.5</v>
       </c>
       <c r="K15" s="4">
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="L15" s="4">
         <v>1.5</v>
       </c>
       <c r="M15" s="4">
-        <v>17.5</v>
+        <v>0</v>
       </c>
       <c r="N15">
         <v>52.5</v>
@@ -2470,10 +2513,10 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="4">
         <v>0</v>
@@ -2497,16 +2540,16 @@
         <v>0</v>
       </c>
       <c r="J16" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="K16" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L16" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M16" s="4">
         <v>4.5</v>
-      </c>
-      <c r="L16" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="M16" s="4">
-        <v>0</v>
       </c>
       <c r="N16">
         <v>36.75</v>
@@ -2516,8 +2559,11 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>84</v>
+      </c>
       <c r="B17" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" s="4">
         <v>0</v>
@@ -2538,19 +2584,19 @@
         <v>0</v>
       </c>
       <c r="I17" s="4">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="J17" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K17" s="4">
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="L17" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="M17" s="4">
-        <v>4.5</v>
+        <v>1.5</v>
       </c>
       <c r="N17">
         <v>78.75</v>
@@ -2560,8 +2606,11 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
       <c r="B18" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C18" s="4">
         <v>0</v>
@@ -2579,16 +2628,16 @@
         <v>0</v>
       </c>
       <c r="H18" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I18" s="4">
-        <v>4.5</v>
+        <v>1.5</v>
       </c>
       <c r="J18" s="4">
         <v>1.5</v>
       </c>
       <c r="K18" s="4">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="L18" s="4">
         <v>0</v>
@@ -2604,8 +2653,11 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
       <c r="B19" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C19" s="4">
         <v>0</v>
@@ -2626,7 +2678,7 @@
         <v>1.5</v>
       </c>
       <c r="I19" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="J19" s="4">
         <v>1.5</v>
@@ -2638,7 +2690,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="4">
-        <v>1.5</v>
+        <v>17.5</v>
       </c>
       <c r="N19">
         <v>82.25</v>
@@ -2648,8 +2700,11 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>84</v>
+      </c>
       <c r="B20" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C20" s="4">
         <v>0</v>
@@ -2667,22 +2722,22 @@
         <v>0</v>
       </c>
       <c r="H20" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="I20" s="4">
         <v>0</v>
       </c>
       <c r="J20" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="K20" s="4">
         <v>0</v>
       </c>
       <c r="L20" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="M20" s="4">
-        <v>17.5</v>
+        <v>9</v>
       </c>
       <c r="N20">
         <v>42</v>
@@ -2692,8 +2747,11 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>84</v>
+      </c>
       <c r="B21" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C21" s="4">
         <v>0</v>
@@ -2705,13 +2763,13 @@
         <v>0</v>
       </c>
       <c r="F21" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G21" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="H21" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I21" s="4">
         <v>0</v>
@@ -2720,13 +2778,13 @@
         <v>0</v>
       </c>
       <c r="K21" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="L21" s="4">
         <v>1.5</v>
       </c>
       <c r="M21" s="4">
-        <v>9</v>
+        <v>17.5</v>
       </c>
       <c r="N21">
         <v>113.75</v>
@@ -2736,8 +2794,11 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>84</v>
+      </c>
       <c r="B22" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C22" s="4">
         <v>0</v>
@@ -2749,7 +2810,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="G22" s="4">
         <v>1.5</v>
@@ -2758,10 +2819,10 @@
         <v>1.5</v>
       </c>
       <c r="I22" s="4">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="J22" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K22" s="4">
         <v>1.5</v>
@@ -2770,7 +2831,7 @@
         <v>1.5</v>
       </c>
       <c r="M22" s="4">
-        <v>17.5</v>
+        <v>4.5</v>
       </c>
       <c r="N22">
         <v>99.75</v>
@@ -2780,8 +2841,11 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>84</v>
+      </c>
       <c r="B23" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C23" s="4">
         <v>0</v>
@@ -2796,25 +2860,25 @@
         <v>0</v>
       </c>
       <c r="G23" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="H23" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="I23" s="4">
-        <v>4.5</v>
+        <v>1.5</v>
       </c>
       <c r="J23" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="K23" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="L23" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="M23" s="4">
-        <v>4.5</v>
+        <v>17.5</v>
       </c>
       <c r="N23">
         <v>71.75</v>
@@ -2824,8 +2888,11 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>84</v>
+      </c>
       <c r="B24" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C24" s="4">
         <v>0</v>
@@ -2849,16 +2916,16 @@
         <v>1.5</v>
       </c>
       <c r="J24" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K24" s="4">
         <v>0</v>
       </c>
       <c r="L24" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="M24" s="4">
-        <v>17.5</v>
+        <v>4.5</v>
       </c>
       <c r="N24">
         <v>47.25</v>
@@ -2868,8 +2935,11 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>84</v>
+      </c>
       <c r="B25" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C25" s="4">
         <v>0</v>
@@ -2890,19 +2960,19 @@
         <v>0</v>
       </c>
       <c r="I25" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="J25" s="4">
         <v>1.5</v>
       </c>
       <c r="K25" s="4">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="L25" s="4">
         <v>1.5</v>
       </c>
       <c r="M25" s="4">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="N25">
         <v>52.5</v>
@@ -2912,8 +2982,11 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>84</v>
+      </c>
       <c r="B26" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C26" s="4">
         <v>0</v>
@@ -2931,22 +3004,22 @@
         <v>0</v>
       </c>
       <c r="H26" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I26" s="4">
         <v>0</v>
       </c>
       <c r="J26" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="K26" s="4">
-        <v>4.5</v>
+        <v>1.5</v>
       </c>
       <c r="L26" s="4">
         <v>1.5</v>
       </c>
       <c r="M26" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="N26">
         <v>36.75</v>
@@ -2956,8 +3029,11 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>85</v>
+      </c>
       <c r="B27" s="4">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C27" s="4">
         <v>0</v>
@@ -2975,19 +3051,19 @@
         <v>0</v>
       </c>
       <c r="H27" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="I27" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="J27" s="4">
         <v>0</v>
       </c>
       <c r="K27" s="4">
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="L27" s="4">
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="M27" s="4">
         <v>1.5</v>
@@ -3001,10 +3077,10 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B28" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" s="4">
         <v>0</v>
@@ -3022,22 +3098,22 @@
         <v>0</v>
       </c>
       <c r="H28" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I28" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="J28" s="4">
         <v>0</v>
       </c>
       <c r="K28" s="4">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="L28" s="4">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="M28" s="4">
-        <v>1.5</v>
+        <v>17.5</v>
       </c>
       <c r="N28">
         <v>71.75</v>
@@ -3047,8 +3123,11 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>85</v>
+      </c>
       <c r="B29" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C29" s="4">
         <v>0</v>
@@ -3066,19 +3145,19 @@
         <v>0</v>
       </c>
       <c r="H29" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="I29" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="J29" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K29" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="L29" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="M29" s="4">
         <v>17.5</v>
@@ -3091,8 +3170,11 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>85</v>
+      </c>
       <c r="B30" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C30" s="4">
         <v>0</v>
@@ -3113,10 +3195,10 @@
         <v>0</v>
       </c>
       <c r="I30" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="J30" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="K30" s="4">
         <v>1.5</v>
@@ -3125,7 +3207,7 @@
         <v>1.5</v>
       </c>
       <c r="M30" s="4">
-        <v>17.5</v>
+        <v>1.5</v>
       </c>
       <c r="N30">
         <v>26.25</v>
@@ -3135,8 +3217,11 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>85</v>
+      </c>
       <c r="B31" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C31" s="4">
         <v>0</v>
@@ -3160,7 +3245,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K31" s="4">
         <v>1.5</v>
@@ -3169,7 +3254,7 @@
         <v>1.5</v>
       </c>
       <c r="M31" s="4">
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="N31">
         <v>47.25</v>
@@ -3179,8 +3264,11 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>85</v>
+      </c>
       <c r="B32" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C32" s="4">
         <v>0</v>
@@ -3213,7 +3301,7 @@
         <v>1.5</v>
       </c>
       <c r="M32" s="4">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="N32">
         <v>31.5</v>
@@ -3223,8 +3311,11 @@
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>85</v>
+      </c>
       <c r="B33" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C33" s="4">
         <v>0</v>
@@ -3248,16 +3339,16 @@
         <v>0</v>
       </c>
       <c r="J33" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="K33" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="L33" s="4">
         <v>1.5</v>
       </c>
       <c r="M33" s="4">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="N33">
         <v>26.25</v>
@@ -3267,8 +3358,11 @@
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>85</v>
+      </c>
       <c r="B34" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C34" s="4">
         <v>0</v>
@@ -3280,28 +3374,28 @@
         <v>0</v>
       </c>
       <c r="F34" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G34" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="H34" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I34" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="J34" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K34" s="4">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="L34" s="4">
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="M34" s="4">
-        <v>4.5</v>
+        <v>62.5</v>
       </c>
       <c r="N34">
         <v>334.25</v>
@@ -3311,8 +3405,11 @@
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>85</v>
+      </c>
       <c r="B35" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C35" s="4">
         <v>0</v>
@@ -3324,13 +3421,13 @@
         <v>0</v>
       </c>
       <c r="F35" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="G35" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="H35" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="I35" s="4">
         <v>1.5</v>
@@ -3339,13 +3436,13 @@
         <v>1.5</v>
       </c>
       <c r="K35" s="4">
-        <v>4.5</v>
+        <v>1.5</v>
       </c>
       <c r="L35" s="4">
-        <v>4.5</v>
+        <v>1.5</v>
       </c>
       <c r="M35" s="4">
-        <v>62.5</v>
+        <v>17.5</v>
       </c>
       <c r="N35">
         <v>103.25</v>
@@ -3355,8 +3452,11 @@
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>85</v>
+      </c>
       <c r="B36" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C36" s="4">
         <v>0</v>
@@ -3374,13 +3474,13 @@
         <v>0</v>
       </c>
       <c r="H36" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I36" s="4">
         <v>1.5</v>
       </c>
       <c r="J36" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="K36" s="4">
         <v>1.5</v>
@@ -3389,7 +3489,7 @@
         <v>1.5</v>
       </c>
       <c r="M36" s="4">
-        <v>17.5</v>
+        <v>0</v>
       </c>
       <c r="N36">
         <v>42</v>
@@ -3399,8 +3499,11 @@
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>85</v>
+      </c>
       <c r="B37" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C37" s="4">
         <v>0</v>
@@ -3418,22 +3521,22 @@
         <v>0</v>
       </c>
       <c r="H37" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="I37" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="J37" s="4">
         <v>0</v>
       </c>
       <c r="K37" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="L37" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="M37" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="N37">
         <v>5.25</v>
@@ -3443,8 +3546,11 @@
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>85</v>
+      </c>
       <c r="B38" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C38" s="4">
         <v>0</v>
@@ -3462,7 +3568,7 @@
         <v>0</v>
       </c>
       <c r="H38" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I38" s="4">
         <v>0</v>
@@ -3477,7 +3583,7 @@
         <v>0</v>
       </c>
       <c r="M38" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="N38">
         <v>10.5</v>
@@ -3487,8 +3593,11 @@
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>86</v>
+      </c>
       <c r="B39" s="4">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C39" s="4">
         <v>0</v>
@@ -3506,7 +3615,7 @@
         <v>0</v>
       </c>
       <c r="H39" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="I39" s="4">
         <v>0</v>
@@ -3532,10 +3641,10 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B40" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C40" s="4">
         <v>0</v>
@@ -3568,7 +3677,7 @@
         <v>0</v>
       </c>
       <c r="M40" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="N40">
         <v>5.25</v>
@@ -3578,8 +3687,11 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>86</v>
+      </c>
       <c r="B41" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C41" s="4">
         <v>0</v>
@@ -3612,7 +3724,7 @@
         <v>0</v>
       </c>
       <c r="M41" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="N41">
         <v>0</v>
@@ -3622,8 +3734,11 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>86</v>
+      </c>
       <c r="B42" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C42" s="4">
         <v>0</v>
@@ -3656,7 +3771,7 @@
         <v>0</v>
       </c>
       <c r="M42" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="N42">
         <v>5.25</v>
@@ -3666,8 +3781,11 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>86</v>
+      </c>
       <c r="B43" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C43" s="4">
         <v>0</v>
@@ -3700,7 +3818,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="N43">
         <v>0</v>
@@ -3710,8 +3828,11 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>86</v>
+      </c>
       <c r="B44" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C44" s="4">
         <v>0</v>
@@ -3754,8 +3875,11 @@
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>86</v>
+      </c>
       <c r="B45" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C45" s="4">
         <v>0</v>
@@ -3798,8 +3922,11 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>86</v>
+      </c>
       <c r="B46" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C46" s="4">
         <v>0</v>
@@ -3842,8 +3969,11 @@
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>86</v>
+      </c>
       <c r="B47" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C47" s="4">
         <v>0</v>
@@ -3886,8 +4016,11 @@
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>86</v>
+      </c>
       <c r="B48" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C48" s="4">
         <v>0</v>
@@ -3920,7 +4053,7 @@
         <v>0</v>
       </c>
       <c r="M48" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="N48">
         <v>5.25</v>
@@ -3929,9 +4062,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>86</v>
+      </c>
       <c r="B49" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C49" s="4">
         <v>0</v>
@@ -3964,7 +4100,7 @@
         <v>0</v>
       </c>
       <c r="M49" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="N49">
         <v>0</v>
@@ -3973,9 +4109,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>86</v>
+      </c>
       <c r="B50" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C50" s="4">
         <v>0</v>
@@ -4014,44 +4153,6 @@
         <v>0</v>
       </c>
       <c r="O50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="4">
-        <v>12</v>
-      </c>
-      <c r="C51" s="4">
-        <v>0</v>
-      </c>
-      <c r="D51" s="4">
-        <v>0</v>
-      </c>
-      <c r="E51" s="4">
-        <v>0</v>
-      </c>
-      <c r="F51" s="4">
-        <v>0</v>
-      </c>
-      <c r="G51" s="4">
-        <v>0</v>
-      </c>
-      <c r="H51" s="4">
-        <v>0</v>
-      </c>
-      <c r="I51" s="4">
-        <v>0</v>
-      </c>
-      <c r="J51" s="4">
-        <v>0</v>
-      </c>
-      <c r="K51" s="4">
-        <v>0</v>
-      </c>
-      <c r="L51" s="4">
-        <v>0</v>
-      </c>
-      <c r="M51" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4072,18 +4173,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" t="s">
         <v>88</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>89</v>
-      </c>
-      <c r="D1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2">
         <v>55.708333333333336</v>
@@ -4097,7 +4198,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3">
         <v>62.5625</v>
@@ -4111,7 +4212,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4">
         <v>73.354166666666671</v>
@@ -4125,7 +4226,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5">
         <v>1.3125</v>

</xml_diff>